<commit_message>
Modificacion base de datos y consultas
</commit_message>
<xml_diff>
--- a/Docs/Seguimiento.xlsx
+++ b/Docs/Seguimiento.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="127">
   <si>
     <t>Colciencias</t>
   </si>
@@ -457,7 +457,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -554,19 +554,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -706,14 +693,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -723,26 +707,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -756,20 +736,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1056,8 +1036,8 @@
   <dimension ref="D1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G79" sqref="G79"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1069,47 +1049,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="H1" s="15" t="s">
+      <c r="H1" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="I1" s="16" t="s">
+      <c r="I1" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="14" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="2" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="33" t="s">
+      <c r="E2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="30" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="3" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="27" t="s">
         <v>117</v>
       </c>
       <c r="E3" s="3" t="s">
@@ -1121,313 +1111,333 @@
       <c r="G3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I3" s="32" t="s">
-        <v>46</v>
-      </c>
-      <c r="J3" s="29" t="s">
-        <v>46</v>
-      </c>
-      <c r="K3" s="34" t="s">
+      <c r="H3" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="29" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="K3" s="31" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="4" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H4" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="25" t="s">
+      <c r="E4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I4" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J4" s="16"/>
+      <c r="K4" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G5" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H5" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I5" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="25" t="s">
+      <c r="E5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="16"/>
+      <c r="K5" s="22" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G6" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="J6" s="19"/>
-      <c r="K6" s="33" t="s">
+      <c r="E6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J6" s="16"/>
+      <c r="K6" s="30" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="7" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G7" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I7" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="26" t="s">
+      <c r="E7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="8" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="33" t="s">
+      <c r="E8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="16"/>
+      <c r="K8" s="30" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="9" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="33" t="s">
+      <c r="E9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H9" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" s="16"/>
+      <c r="K9" s="30" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="10" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E10" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H10" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" s="31" t="s">
+      <c r="E10" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I10" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J10" s="2"/>
-      <c r="K10" s="27" t="s">
+      <c r="K10" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="11" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E11" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G11" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H11" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I11" s="31" t="s">
+      <c r="E11" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J11" s="2"/>
-      <c r="K11" s="27" t="s">
+      <c r="K11" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I12" s="31" t="s">
+      <c r="E12" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I12" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J12" s="2"/>
-      <c r="K12" s="34" t="s">
+      <c r="K12" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="13" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" s="31" t="s">
+      <c r="E13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H13" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J13" s="2"/>
-      <c r="K13" s="27" t="s">
+      <c r="K13" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E14" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I14" s="31" t="s">
+      <c r="E14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H14" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J14" s="2"/>
-      <c r="K14" s="27" t="s">
+      <c r="K14" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E15" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G15" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H15" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I15" s="31" t="s">
+      <c r="E15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H15" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J15" s="2"/>
-      <c r="K15" s="27" t="s">
+      <c r="K15" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G16" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H16" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I16" s="31" t="s">
+      <c r="E16" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H16" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I16" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J16" s="2"/>
-      <c r="K16" s="27" t="s">
+      <c r="K16" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D17" s="8" t="s">
+      <c r="D17" s="7" t="s">
         <v>13</v>
       </c>
       <c r="E17" s="2" t="s">
@@ -1445,15 +1455,15 @@
       <c r="I17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="19" t="s">
-        <v>46</v>
-      </c>
-      <c r="K17" s="33" t="s">
+      <c r="J17" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="30" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="18" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E18" s="2" t="s">
@@ -1471,13 +1481,13 @@
       <c r="I18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="33" t="s">
+      <c r="J18" s="16"/>
+      <c r="K18" s="30" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="19" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E19" s="2" t="s">
@@ -1496,26 +1506,36 @@
         <v>46</v>
       </c>
       <c r="J19" s="2"/>
-      <c r="K19" s="33" t="s">
+      <c r="K19" s="30" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="E20" s="24"/>
-      <c r="F20" s="24"/>
-      <c r="G20" s="24"/>
-      <c r="H20" s="24"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="35" t="s">
+      <c r="E20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="21"/>
+      <c r="K20" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="21" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>16</v>
       </c>
       <c r="E21" s="2" t="s">
@@ -1533,13 +1553,13 @@
       <c r="I21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J21" s="24"/>
-      <c r="K21" s="35" t="s">
+      <c r="J21" s="21"/>
+      <c r="K21" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>17</v>
       </c>
       <c r="E22" s="2" t="s">
@@ -1557,19 +1577,19 @@
       <c r="I22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J22" s="24"/>
-      <c r="K22" s="35" t="s">
+      <c r="J22" s="21"/>
+      <c r="K22" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="23" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E23" s="24" t="s">
-        <v>37</v>
-      </c>
-      <c r="F23" s="24" t="s">
+      <c r="E23" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F23" s="21" t="s">
         <v>46</v>
       </c>
       <c r="G23" s="2" t="s">
@@ -1581,177 +1601,277 @@
       <c r="I23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J23" s="24"/>
-      <c r="K23" s="35" t="s">
+      <c r="J23" s="21"/>
+      <c r="K23" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="24" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="35" t="s">
+      <c r="E24" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J24" s="21"/>
+      <c r="K24" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="25" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="35" t="s">
+      <c r="E25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J25" s="21"/>
+      <c r="K25" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="26" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="24"/>
-      <c r="F26" s="24"/>
-      <c r="G26" s="24"/>
-      <c r="H26" s="24"/>
-      <c r="I26" s="24"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="35" t="s">
+      <c r="E26" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F26" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J26" s="21"/>
+      <c r="K26" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="27" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="24"/>
-      <c r="F27" s="24"/>
-      <c r="G27" s="24"/>
-      <c r="H27" s="24"/>
-      <c r="I27" s="24"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="35" t="s">
+      <c r="E27" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F27" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J27" s="21"/>
+      <c r="K27" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="28" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="24"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="24"/>
-      <c r="I28" s="24"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="35" t="s">
+      <c r="E28" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F28" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J28" s="21"/>
+      <c r="K28" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="29" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E29" s="24"/>
-      <c r="F29" s="24"/>
-      <c r="G29" s="24"/>
-      <c r="H29" s="24"/>
-      <c r="I29" s="24"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="35" t="s">
+      <c r="E29" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J29" s="21"/>
+      <c r="K29" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="30" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="24"/>
-      <c r="F30" s="24"/>
-      <c r="G30" s="24"/>
-      <c r="H30" s="24"/>
-      <c r="I30" s="24"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="35" t="s">
+      <c r="E30" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J30" s="21"/>
+      <c r="K30" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="31" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E31" s="24"/>
-      <c r="F31" s="24"/>
-      <c r="G31" s="24"/>
-      <c r="H31" s="24"/>
-      <c r="I31" s="24"/>
-      <c r="J31" s="24"/>
-      <c r="K31" s="35" t="s">
+      <c r="E31" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J31" s="21"/>
+      <c r="K31" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="32" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E32" s="24"/>
-      <c r="F32" s="24"/>
-      <c r="G32" s="24"/>
-      <c r="H32" s="24"/>
-      <c r="I32" s="24"/>
-      <c r="J32" s="24"/>
-      <c r="K32" s="35" t="s">
+      <c r="E32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F32" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J32" s="21"/>
+      <c r="K32" s="32" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="33" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
+      <c r="E33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J33" s="2"/>
-      <c r="K33" s="27" t="s">
+      <c r="K33" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E34" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F34" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G34" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H34" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I34" s="31" t="s">
+      <c r="E34" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I34" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J34" s="2"/>
-      <c r="K34" s="27" t="s">
+      <c r="K34" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="6" t="s">
         <v>56</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -1769,13 +1889,13 @@
       <c r="I35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J35" s="20"/>
-      <c r="K35" s="33" t="s">
+      <c r="J35" s="17"/>
+      <c r="K35" s="30" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="36" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="6" t="s">
         <v>57</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -1794,40 +1914,60 @@
         <v>46</v>
       </c>
       <c r="J36" s="2"/>
-      <c r="K36" s="33" t="s">
+      <c r="K36" s="30" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="37" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="21"/>
-      <c r="K37" s="33" t="s">
+      <c r="E37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="18"/>
+      <c r="K37" s="30" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="38" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="21"/>
-      <c r="K38" s="33" t="s">
+      <c r="E38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J38" s="18"/>
+      <c r="K38" s="30" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -1845,57 +1985,87 @@
       <c r="I39" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J39" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K39" s="33" t="s">
+      <c r="J39" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K39" s="30" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="40" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="21"/>
-      <c r="K40" s="33" t="s">
+      <c r="E40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J40" s="18"/>
+      <c r="K40" s="30" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="41" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="21"/>
-      <c r="K41" s="33" t="s">
+      <c r="E41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J41" s="18"/>
+      <c r="K41" s="30" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="42" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="21"/>
-      <c r="K42" s="33" t="s">
+      <c r="E42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J42" s="18"/>
+      <c r="K42" s="30" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="43" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="6" t="s">
         <v>63</v>
       </c>
       <c r="E43" s="3" t="s">
@@ -1911,39 +2081,39 @@
       <c r="I43" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J43" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K43" s="33" t="s">
+      <c r="J43" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K43" s="30" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="44" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F44" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G44" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H44" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I44" s="31" t="s">
+      <c r="E44" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H44" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I44" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J44" s="2"/>
-      <c r="K44" s="27" t="s">
+      <c r="K44" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="45" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="6" t="s">
         <v>65</v>
       </c>
       <c r="E45" s="3" t="s">
@@ -1959,15 +2129,15 @@
       <c r="I45" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="J45" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K45" s="33" t="s">
+      <c r="J45" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K45" s="30" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="46" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="6" t="s">
         <v>66</v>
       </c>
       <c r="E46" s="3" t="s">
@@ -1983,15 +2153,15 @@
       <c r="I46" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J46" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K46" s="33" t="s">
+      <c r="J46" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K46" s="30" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="47" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D47" s="7" t="s">
+      <c r="D47" s="6" t="s">
         <v>67</v>
       </c>
       <c r="E47" s="3" t="s">
@@ -2007,13 +2177,13 @@
       <c r="I47" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J47" s="21"/>
-      <c r="K47" s="33" t="s">
+      <c r="J47" s="18"/>
+      <c r="K47" s="30" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="48" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D48" s="7" t="s">
+      <c r="D48" s="6" t="s">
         <v>121</v>
       </c>
       <c r="E48" s="3" t="s">
@@ -2029,83 +2199,111 @@
       <c r="I48" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J48" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K48" s="34" t="s">
+      <c r="J48" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K48" s="31" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="49" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F49" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G49" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H49" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I49" s="31" t="s">
+      <c r="E49" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G49" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I49" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J49" s="2"/>
-      <c r="K49" s="27" t="s">
+      <c r="K49" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="6" t="s">
         <v>23</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F50" s="2"/>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
+      <c r="F50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H50" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I50" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="J50" s="2"/>
-      <c r="K50" s="34" t="s">
+      <c r="K50" s="31" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="51" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
+      <c r="E51" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H51" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I51" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="J51" s="2"/>
-      <c r="K51" s="34" t="s">
+      <c r="K51" s="31" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="52" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
+      <c r="E52" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H52" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I52" s="28" t="s">
+        <v>46</v>
+      </c>
       <c r="J52" s="2"/>
-      <c r="K52" s="34" t="s">
+      <c r="K52" s="31" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="53" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="6" t="s">
         <v>95</v>
       </c>
       <c r="E53" s="3" t="s">
@@ -2123,41 +2321,61 @@
       <c r="I53" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J53" s="20"/>
-      <c r="K53" s="33" t="s">
+      <c r="J53" s="17"/>
+      <c r="K53" s="30" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="54" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
+      <c r="E54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J54" s="2"/>
-      <c r="K54" s="34" t="s">
+      <c r="K54" s="31" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="55" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
+      <c r="E55" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J55" s="2"/>
-      <c r="K55" s="34" t="s">
+      <c r="K55" s="31" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="56" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E56" s="3" t="s">
@@ -2178,36 +2396,36 @@
       <c r="J56" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="K56" s="33" t="s">
+      <c r="K56" s="30" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="57" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E57" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F57" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G57" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H57" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I57" s="31" t="s">
+      <c r="E57" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G57" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H57" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I57" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J57" s="2"/>
-      <c r="K57" s="34" t="s">
+      <c r="K57" s="31" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="58" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="6" t="s">
         <v>42</v>
       </c>
       <c r="E58" s="2" t="s">
@@ -2225,13 +2443,13 @@
       <c r="I58" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="J58" s="21"/>
-      <c r="K58" s="33" t="s">
+      <c r="J58" s="18"/>
+      <c r="K58" s="30" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="59" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="6" t="s">
         <v>43</v>
       </c>
       <c r="E59" s="3" t="s">
@@ -2249,65 +2467,85 @@
       <c r="I59" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J59" s="21"/>
-      <c r="K59" s="33" t="s">
+      <c r="J59" s="18"/>
+      <c r="K59" s="30" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="60" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="21"/>
-      <c r="K60" s="33" t="s">
+      <c r="E60" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J60" s="18"/>
+      <c r="K60" s="30" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="61" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="21"/>
-      <c r="K61" s="33" t="s">
+      <c r="E61" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J61" s="18"/>
+      <c r="K61" s="30" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="62" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E62" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F62" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G62" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H62" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I62" s="31" t="s">
+      <c r="E62" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G62" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H62" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I62" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J62" s="2"/>
-      <c r="K62" s="27" t="s">
+      <c r="K62" s="24" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="63" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="6" t="s">
         <v>47</v>
       </c>
       <c r="E63" s="3"/>
@@ -2315,13 +2553,13 @@
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
       <c r="I63" s="3"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="33" t="s">
+      <c r="J63" s="18"/>
+      <c r="K63" s="30" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="64" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D64" s="7" t="s">
+      <c r="D64" s="6" t="s">
         <v>48</v>
       </c>
       <c r="E64" s="3"/>
@@ -2329,13 +2567,13 @@
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
       <c r="I64" s="3"/>
-      <c r="J64" s="21"/>
-      <c r="K64" s="33" t="s">
+      <c r="J64" s="18"/>
+      <c r="K64" s="30" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="65" spans="4:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="6" t="s">
         <v>49</v>
       </c>
       <c r="E65" s="3"/>
@@ -2343,13 +2581,13 @@
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
       <c r="I65" s="3"/>
-      <c r="J65" s="21"/>
-      <c r="K65" s="33" t="s">
+      <c r="J65" s="18"/>
+      <c r="K65" s="30" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="66" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D66" s="7" t="s">
+      <c r="D66" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E66" s="3"/>
@@ -2357,67 +2595,85 @@
       <c r="G66" s="3"/>
       <c r="H66" s="3"/>
       <c r="I66" s="3"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="33" t="s">
+      <c r="J66" s="18"/>
+      <c r="K66" s="30" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="67" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E67" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="F67" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G67" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="H67" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="I67" s="31" t="s">
+      <c r="E67" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F67" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="G67" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="H67" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="I67" s="28" t="s">
         <v>46</v>
       </c>
       <c r="J67" s="2"/>
-      <c r="K67" s="26" t="s">
+      <c r="K67" s="23" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="68" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D68" s="7" t="s">
+      <c r="D68" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
-      <c r="J68" s="21"/>
-      <c r="K68" s="33" t="s">
+      <c r="E68" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I68" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J68" s="18"/>
+      <c r="K68" s="30" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="69" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D69" s="7" t="s">
+      <c r="D69" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
-      <c r="J69" s="21"/>
-      <c r="K69" s="33" t="s">
+      <c r="F69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="J69" s="18"/>
+      <c r="K69" s="30" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="70" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D70" s="7" t="s">
+      <c r="D70" s="6" t="s">
         <v>108</v>
       </c>
       <c r="E70" s="3" t="s">
@@ -2435,13 +2691,13 @@
       <c r="I70" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J70" s="21"/>
-      <c r="K70" s="33" t="s">
+      <c r="J70" s="18"/>
+      <c r="K70" s="30" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="71" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D71" s="7" t="s">
+      <c r="D71" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E71" s="3" t="s">
@@ -2459,13 +2715,13 @@
       <c r="I71" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J71" s="21"/>
-      <c r="K71" s="33" t="s">
+      <c r="J71" s="18"/>
+      <c r="K71" s="30" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="72" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D72" s="7" t="s">
+      <c r="D72" s="6" t="s">
         <v>52</v>
       </c>
       <c r="E72" s="3" t="s">
@@ -2483,53 +2739,53 @@
       <c r="I72" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="J72" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="K72" s="33" t="s">
+      <c r="J72" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="K72" s="30" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="73" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D73" s="9" t="s">
+      <c r="D73" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E73" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F73" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H73" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I73" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="J73" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="K73" s="36" t="s">
+      <c r="E73" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F73" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="G73" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="H73" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I73" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J73" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="K73" s="33" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="74" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="K74" s="28"/>
+      <c r="K74" s="25"/>
     </row>
     <row r="75" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="K75" s="28"/>
+      <c r="K75" s="25"/>
     </row>
     <row r="76" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="K76" s="28"/>
+      <c r="K76" s="25"/>
     </row>
     <row r="77" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="K77" s="28"/>
+      <c r="K77" s="25"/>
     </row>
     <row r="78" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="K78" s="28"/>
+      <c r="K78" s="25"/>
     </row>
     <row r="79" spans="4:11" x14ac:dyDescent="0.25">
       <c r="G79" s="1"/>

</xml_diff>

<commit_message>
Cambio base de datos
</commit_message>
<xml_diff>
--- a/Docs/Seguimiento.xlsx
+++ b/Docs/Seguimiento.xlsx
@@ -15,6 +15,7 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="127">
   <si>
     <t>Colciencias</t>
   </si>
@@ -1037,7 +1038,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I58" sqref="I58"/>
+      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,11 +2549,21 @@
       <c r="D63" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
+      <c r="E63" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H63" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="J63" s="18"/>
       <c r="K63" s="30" t="s">
         <v>102</v>

</xml_diff>

<commit_message>
Cambios por modificaciones de la base de datos
</commit_message>
<xml_diff>
--- a/Docs/Seguimiento.xlsx
+++ b/Docs/Seguimiento.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="128">
   <si>
     <t>Colciencias</t>
   </si>
@@ -406,6 +405,9 @@
   </si>
   <si>
     <t>http://localhost/SIGPYS/Views/resultadoDiseno.php</t>
+  </si>
+  <si>
+    <t>Hace falta revisar la consulta por los proyectos y solicitudes especificas que muestra</t>
   </si>
 </sst>
 </file>
@@ -694,7 +696,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -751,6 +753,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1037,8 +1042,8 @@
   <dimension ref="D1:K99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E64" sqref="E64"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1099,7 +1104,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="4:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="4:11" ht="30" x14ac:dyDescent="0.25">
       <c r="D3" s="27" t="s">
         <v>117</v>
       </c>
@@ -1115,8 +1120,8 @@
       <c r="H3" s="28" t="s">
         <v>46</v>
       </c>
-      <c r="I3" s="29" t="s">
-        <v>46</v>
+      <c r="I3" s="34" t="s">
+        <v>127</v>
       </c>
       <c r="J3" s="26" t="s">
         <v>46</v>
@@ -2573,11 +2578,21 @@
       <c r="D64" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
+      <c r="E64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J64" s="18"/>
       <c r="K64" s="30" t="s">
         <v>103</v>
@@ -2587,11 +2602,21 @@
       <c r="D65" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
+      <c r="E65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J65" s="18"/>
       <c r="K65" s="30" t="s">
         <v>104</v>
@@ -2601,11 +2626,21 @@
       <c r="D66" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
+      <c r="E66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>46</v>
+      </c>
       <c r="J66" s="18"/>
       <c r="K66" s="30" t="s">
         <v>105</v>

</xml_diff>